<commit_message>
update of output excels
</commit_message>
<xml_diff>
--- a/data_processed/20250620/BTCUSDVOLSURFACE_20250620.xlsx
+++ b/data_processed/20250620/BTCUSDVOLSURFACE_20250620.xlsx
@@ -1684,7 +1684,7 @@
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>BF,CA</t>
+          <t>CA,BF</t>
         </is>
       </c>
     </row>
@@ -2989,7 +2989,7 @@
       </c>
       <c r="G88" t="inlineStr">
         <is>
-          <t>BF,CA</t>
+          <t>CA,BF</t>
         </is>
       </c>
     </row>
@@ -3685,7 +3685,7 @@
       </c>
       <c r="G112" t="inlineStr">
         <is>
-          <t>BF,CA</t>
+          <t>CA,BF</t>
         </is>
       </c>
     </row>
@@ -4207,7 +4207,7 @@
       </c>
       <c r="G130" t="inlineStr">
         <is>
-          <t>BF,CA</t>
+          <t>CA,BF</t>
         </is>
       </c>
     </row>
@@ -4555,7 +4555,7 @@
       </c>
       <c r="G142" t="inlineStr">
         <is>
-          <t>BF,CA</t>
+          <t>CA,BF</t>
         </is>
       </c>
     </row>
@@ -4584,7 +4584,7 @@
       </c>
       <c r="G143" t="inlineStr">
         <is>
-          <t>BF,CA</t>
+          <t>CA,BF</t>
         </is>
       </c>
     </row>
@@ -4990,7 +4990,7 @@
       </c>
       <c r="G157" t="inlineStr">
         <is>
-          <t>BF,CA</t>
+          <t>CA,BF</t>
         </is>
       </c>
     </row>
@@ -5367,7 +5367,7 @@
       </c>
       <c r="G170" t="inlineStr">
         <is>
-          <t>BF,CA</t>
+          <t>CA,BF</t>
         </is>
       </c>
     </row>
@@ -5715,7 +5715,7 @@
       </c>
       <c r="G182" t="inlineStr">
         <is>
-          <t>BF,CA</t>
+          <t>CA,BF</t>
         </is>
       </c>
     </row>
@@ -6005,7 +6005,7 @@
       </c>
       <c r="G192" t="inlineStr">
         <is>
-          <t>BF,CA</t>
+          <t>CA,BF</t>
         </is>
       </c>
     </row>
@@ -6179,7 +6179,7 @@
       </c>
       <c r="G198" t="inlineStr">
         <is>
-          <t>BF,CA</t>
+          <t>CA,BF</t>
         </is>
       </c>
     </row>
@@ -6208,7 +6208,7 @@
       </c>
       <c r="G199" t="inlineStr">
         <is>
-          <t>BF,CA</t>
+          <t>CA,BF</t>
         </is>
       </c>
     </row>
@@ -6411,7 +6411,7 @@
       </c>
       <c r="G206" t="inlineStr">
         <is>
-          <t>BF,CA</t>
+          <t>CA,BF</t>
         </is>
       </c>
     </row>
@@ -6440,7 +6440,7 @@
       </c>
       <c r="G207" t="inlineStr">
         <is>
-          <t>BF,CA</t>
+          <t>CA,BF</t>
         </is>
       </c>
     </row>
@@ -6701,7 +6701,7 @@
       </c>
       <c r="G216" t="inlineStr">
         <is>
-          <t>BF,CA</t>
+          <t>CA,BF</t>
         </is>
       </c>
     </row>
@@ -6730,7 +6730,7 @@
       </c>
       <c r="G217" t="inlineStr">
         <is>
-          <t>BF,CA</t>
+          <t>CA,BF</t>
         </is>
       </c>
     </row>
@@ -6991,7 +6991,7 @@
       </c>
       <c r="G226" t="inlineStr">
         <is>
-          <t>BF,CA</t>
+          <t>CA,BF</t>
         </is>
       </c>
     </row>
@@ -7165,7 +7165,7 @@
       </c>
       <c r="G232" t="inlineStr">
         <is>
-          <t>BF,CA</t>
+          <t>CA,BF</t>
         </is>
       </c>
     </row>
@@ -7194,7 +7194,7 @@
       </c>
       <c r="G233" t="inlineStr">
         <is>
-          <t>BF,CA</t>
+          <t>CA,BF</t>
         </is>
       </c>
     </row>
@@ -7339,7 +7339,7 @@
       </c>
       <c r="G238" t="inlineStr">
         <is>
-          <t>BF,CA</t>
+          <t>CA,BF</t>
         </is>
       </c>
     </row>
@@ -7368,7 +7368,7 @@
       </c>
       <c r="G239" t="inlineStr">
         <is>
-          <t>BF,CA</t>
+          <t>CA,BF</t>
         </is>
       </c>
     </row>
@@ -15305,7 +15305,7 @@
       </c>
       <c r="G524" t="inlineStr">
         <is>
-          <t>BF,CA</t>
+          <t>CA,BF</t>
         </is>
       </c>
     </row>
@@ -15595,7 +15595,7 @@
       </c>
       <c r="G534" t="inlineStr">
         <is>
-          <t>BF,CA</t>
+          <t>CA,BF</t>
         </is>
       </c>
     </row>
@@ -15856,7 +15856,7 @@
       </c>
       <c r="G543" t="inlineStr">
         <is>
-          <t>BF,CA</t>
+          <t>CA,BF</t>
         </is>
       </c>
     </row>
@@ -15885,7 +15885,7 @@
       </c>
       <c r="G544" t="inlineStr">
         <is>
-          <t>BF,CA</t>
+          <t>CA,BF</t>
         </is>
       </c>
     </row>
@@ -16146,7 +16146,7 @@
       </c>
       <c r="G553" t="inlineStr">
         <is>
-          <t>BF,CA</t>
+          <t>CA,BF</t>
         </is>
       </c>
     </row>
@@ -16175,7 +16175,7 @@
       </c>
       <c r="G554" t="inlineStr">
         <is>
-          <t>BF,CA</t>
+          <t>CA,BF</t>
         </is>
       </c>
     </row>
@@ -16407,7 +16407,7 @@
       </c>
       <c r="G562" t="inlineStr">
         <is>
-          <t>BF,CA</t>
+          <t>CA,BF</t>
         </is>
       </c>
     </row>
@@ -16436,7 +16436,7 @@
       </c>
       <c r="G563" t="inlineStr">
         <is>
-          <t>BF,CA</t>
+          <t>CA,BF</t>
         </is>
       </c>
     </row>
@@ -16871,7 +16871,7 @@
       </c>
       <c r="G578" t="inlineStr">
         <is>
-          <t>BF,CA</t>
+          <t>CA,BF</t>
         </is>
       </c>
     </row>
@@ -16900,7 +16900,7 @@
       </c>
       <c r="G579" t="inlineStr">
         <is>
-          <t>BF,CA</t>
+          <t>CA,BF</t>
         </is>
       </c>
     </row>
@@ -17393,7 +17393,7 @@
       </c>
       <c r="G596" t="inlineStr">
         <is>
-          <t>BF,CA</t>
+          <t>CA,BF</t>
         </is>
       </c>
     </row>
@@ -17422,7 +17422,7 @@
       </c>
       <c r="G597" t="inlineStr">
         <is>
-          <t>BF,CA</t>
+          <t>CA,BF</t>
         </is>
       </c>
     </row>
@@ -17828,7 +17828,7 @@
       </c>
       <c r="G611" t="inlineStr">
         <is>
-          <t>BF,CA</t>
+          <t>CA,BF</t>
         </is>
       </c>
     </row>
@@ -18118,7 +18118,7 @@
       </c>
       <c r="G621" t="inlineStr">
         <is>
-          <t>BF,CA</t>
+          <t>CA,BF</t>
         </is>
       </c>
     </row>
@@ -18408,7 +18408,7 @@
       </c>
       <c r="G631" t="inlineStr">
         <is>
-          <t>BF,CA</t>
+          <t>CA,BF</t>
         </is>
       </c>
     </row>
@@ -18640,7 +18640,7 @@
       </c>
       <c r="G639" t="inlineStr">
         <is>
-          <t>BF,CA</t>
+          <t>CA,BF</t>
         </is>
       </c>
     </row>
@@ -18872,7 +18872,7 @@
       </c>
       <c r="G647" t="inlineStr">
         <is>
-          <t>BF,CA</t>
+          <t>CA,BF</t>
         </is>
       </c>
     </row>
@@ -19104,7 +19104,7 @@
       </c>
       <c r="G655" t="inlineStr">
         <is>
-          <t>BF,CA</t>
+          <t>CA,BF</t>
         </is>
       </c>
     </row>
@@ -19278,7 +19278,7 @@
       </c>
       <c r="G661" t="inlineStr">
         <is>
-          <t>BF,CA</t>
+          <t>CA,BF</t>
         </is>
       </c>
     </row>
@@ -19307,7 +19307,7 @@
       </c>
       <c r="G662" t="inlineStr">
         <is>
-          <t>BF,CA</t>
+          <t>CA,BF</t>
         </is>
       </c>
     </row>
@@ -19539,7 +19539,7 @@
       </c>
       <c r="G670" t="inlineStr">
         <is>
-          <t>BF,CA</t>
+          <t>CA,BF</t>
         </is>
       </c>
     </row>
@@ -19771,7 +19771,7 @@
       </c>
       <c r="G678" t="inlineStr">
         <is>
-          <t>BF,CA</t>
+          <t>CA,BF</t>
         </is>
       </c>
     </row>
@@ -19974,7 +19974,7 @@
       </c>
       <c r="G685" t="inlineStr">
         <is>
-          <t>BF,CA</t>
+          <t>CA,BF</t>
         </is>
       </c>
     </row>
@@ -20003,7 +20003,7 @@
       </c>
       <c r="G686" t="inlineStr">
         <is>
-          <t>BF,CA</t>
+          <t>CA,BF</t>
         </is>
       </c>
     </row>
@@ -20235,7 +20235,7 @@
       </c>
       <c r="G694" t="inlineStr">
         <is>
-          <t>BF,CA</t>
+          <t>CA,BF</t>
         </is>
       </c>
     </row>
@@ -20380,7 +20380,7 @@
       </c>
       <c r="G699" t="inlineStr">
         <is>
-          <t>BF,CA</t>
+          <t>CA,BF</t>
         </is>
       </c>
     </row>
@@ -20409,7 +20409,7 @@
       </c>
       <c r="G700" t="inlineStr">
         <is>
-          <t>BF,CA</t>
+          <t>CA,BF</t>
         </is>
       </c>
     </row>
@@ -20612,7 +20612,7 @@
       </c>
       <c r="G707" t="inlineStr">
         <is>
-          <t>BF,CA</t>
+          <t>CA,BF</t>
         </is>
       </c>
     </row>
@@ -20786,7 +20786,7 @@
       </c>
       <c r="G713" t="inlineStr">
         <is>
-          <t>BF,CA</t>
+          <t>CA,BF</t>
         </is>
       </c>
     </row>
@@ -20902,7 +20902,7 @@
       </c>
       <c r="G717" t="inlineStr">
         <is>
-          <t>BF,CA</t>
+          <t>CA,BF</t>
         </is>
       </c>
     </row>
@@ -25568,7 +25568,7 @@
       </c>
       <c r="G891" t="inlineStr">
         <is>
-          <t>BF,CA</t>
+          <t>CA,BF</t>
         </is>
       </c>
     </row>
@@ -25713,7 +25713,7 @@
       </c>
       <c r="G896" t="inlineStr">
         <is>
-          <t>BF,CA</t>
+          <t>CA,BF</t>
         </is>
       </c>
     </row>
@@ -25800,7 +25800,7 @@
       </c>
       <c r="G899" t="inlineStr">
         <is>
-          <t>BF,CA</t>
+          <t>CA,BF</t>
         </is>
       </c>
     </row>
@@ -25945,7 +25945,7 @@
       </c>
       <c r="G904" t="inlineStr">
         <is>
-          <t>BF,CA</t>
+          <t>CA,BF</t>
         </is>
       </c>
     </row>
@@ -26003,7 +26003,7 @@
       </c>
       <c r="G906" t="inlineStr">
         <is>
-          <t>BF,CA</t>
+          <t>CA,BF</t>
         </is>
       </c>
     </row>
@@ -26061,7 +26061,7 @@
       </c>
       <c r="G908" t="inlineStr">
         <is>
-          <t>BF,CA</t>
+          <t>CA,BF</t>
         </is>
       </c>
     </row>
@@ -58534,7 +58534,7 @@
       </c>
       <c r="G2161" t="inlineStr">
         <is>
-          <t>BF,CA</t>
+          <t>CA,BF</t>
         </is>
       </c>
     </row>
@@ -58621,7 +58621,7 @@
       </c>
       <c r="G2164" t="inlineStr">
         <is>
-          <t>BF,CA</t>
+          <t>CA,BF</t>
         </is>
       </c>
     </row>

</xml_diff>